<commit_message>
reorganizing git and drift images
</commit_message>
<xml_diff>
--- a/DataAnalysis/FrequencyDrift2021-07-21noscan.xlsx
+++ b/DataAnalysis/FrequencyDrift2021-07-21noscan.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottezehnder/Documents/Academic/Summer 2021 Phys REU/laserStabilization/DataAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4B4B17B8-CE37-2F4B-9AD8-8143D181348C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4944143C-47BA-4142-9FB8-D67B95EAC34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="460" windowWidth="27680" windowHeight="15740"/>
+    <workbookView xWindow="0" yWindow="8240" windowWidth="27680" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FrequencyDrift2021-07-21noscan" sheetId="1" r:id="rId1"/>
@@ -37,13 +37,13 @@
     <t xml:space="preserve"> Active Current (mA) </t>
   </si>
   <si>
-    <t xml:space="preserve"> Frequency Drift (MHz)</t>
+    <t xml:space="preserve"> Frequency Drift (GHz)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -640,7 +640,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> Frequency Drift (MHz)</c:v>
+                  <c:v> Frequency Drift (GHz)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -681,6 +681,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.7028703341315693E-4"/>
+                  <c:y val="6.4061942257217841E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1283,6 +1289,672 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28107633420822398"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'FrequencyDrift2021-07-21noscan'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Active Current (mA) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'FrequencyDrift2021-07-21noscan'!$A$2:$A$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>2.3279999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.658000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.991999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.314</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63.643000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78.995999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>94.325000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>109.654</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124.98099999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140.30799999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>155.63499999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>170.971</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>186.29499999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>201.62200000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>216.94399999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>232.28100000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>247.61</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>262.94</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>278.26799999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>293.62</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>308.93599999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>324.26100000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>339.59</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>354.92099999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>370.262</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>385.59199999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>400.91</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>416.24799999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>431.56900000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>446.91</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>462.23700000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>477.55799999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>492.88600000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>508.221</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>523.54300000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>538.86300000000006</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>554.20899999999995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>569.53300000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>584.84500000000003</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>600.18200000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>615.495</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>630.81700000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>646.15300000000002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>661.48900000000003</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>676.81299999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>692.14</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>707.46799999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>722.79499999999996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>738.11599999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>753.44500000000005</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>768.78099999999995</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>784.10900000000004</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>799.44299999999998</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>814.77099999999996</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>830.10699999999997</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>845.43200000000002</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>860.75599999999997</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>876.08600000000001</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>891.41399999999999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>906.74199999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'FrequencyDrift2021-07-21noscan'!$C$2:$C$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.177133443163</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128.177133443163</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.177133443163</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>128.13495881383801</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>128.168698517298</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>128.177133443163</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128.168698517298</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>128.177133443163</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>128.118088962108</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>128.19400329489201</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>128.168698517298</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>128.12652388797301</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>128.13495881383801</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>128.177133443163</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>128.168698517298</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>128.12652388797301</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>128.13495881383801</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>128.168698517298</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>128.168698517298</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>128.168698517298</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>128.13495881383801</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>128.185568369028</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>128.15182866556799</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>128.118088962108</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>128.185568369028</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>128.16026359143299</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>128.14339373970299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DBAA-9048-BAC2-E9E2057D9344}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1725414960"/>
+        <c:axId val="1725882816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1725414960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1725882816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1725882816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1725414960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1323,7 +1995,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1872,6 +3100,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F544FED-DC1B-194F-BE7B-B0F1F5A61D4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2176,11 +3440,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>